<commit_message>
[WIP] Added REPCA1 model; added `service.CurrentSign`
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_reg.xlsx
+++ b/andes/cases/kundur/kundur_reg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635F6888-1C51-3748-8150-0A81249728CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1E2AFB-0E64-2541-B46B-95BDB882981B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39200" yWindow="1640" windowWidth="27400" windowHeight="16380" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15780" yWindow="7900" windowWidth="30260" windowHeight="19240" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,18 @@
     <sheet name="GENROU" sheetId="7" r:id="rId7"/>
     <sheet name="TGOV1" sheetId="8" r:id="rId8"/>
     <sheet name="EXDC2" sheetId="9" r:id="rId9"/>
-    <sheet name="REGCA1" sheetId="10" r:id="rId10"/>
-    <sheet name="REECA1" sheetId="11" r:id="rId11"/>
-    <sheet name="Toggler" sheetId="12" r:id="rId12"/>
+    <sheet name="BusFreq" sheetId="10" r:id="rId10"/>
+    <sheet name="REGCA1" sheetId="11" r:id="rId11"/>
+    <sheet name="REECA1" sheetId="12" r:id="rId12"/>
+    <sheet name="REPCA1" sheetId="13" r:id="rId13"/>
+    <sheet name="Toggler" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="212">
   <si>
     <t>idx</t>
   </si>
@@ -366,6 +368,15 @@
     <t>EXDC2_3</t>
   </si>
   <si>
+    <t>Tf</t>
+  </si>
+  <si>
+    <t>Tw</t>
+  </si>
+  <si>
+    <t>BusFreq_1</t>
+  </si>
+  <si>
     <t>Tg</t>
   </si>
   <si>
@@ -492,6 +503,9 @@
     <t>Kvi</t>
   </si>
   <si>
+    <t>Vref1</t>
+  </si>
+  <si>
     <t>Tiq</t>
   </si>
   <si>
@@ -564,6 +578,81 @@
     <t>REECA1_1</t>
   </si>
   <si>
+    <t>ree</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>busf</t>
+  </si>
+  <si>
+    <t>Kp</t>
+  </si>
+  <si>
+    <t>Ki</t>
+  </si>
+  <si>
+    <t>Tft</t>
+  </si>
+  <si>
+    <t>Tfv</t>
+  </si>
+  <si>
+    <t>Vfrz</t>
+  </si>
+  <si>
+    <t>Rc</t>
+  </si>
+  <si>
+    <t>Xc</t>
+  </si>
+  <si>
+    <t>emax</t>
+  </si>
+  <si>
+    <t>emin</t>
+  </si>
+  <si>
+    <t>Qmax</t>
+  </si>
+  <si>
+    <t>Qmin</t>
+  </si>
+  <si>
+    <t>Kpg</t>
+  </si>
+  <si>
+    <t>Kig</t>
+  </si>
+  <si>
+    <t>fdbd1</t>
+  </si>
+  <si>
+    <t>fdbd2</t>
+  </si>
+  <si>
+    <t>femax</t>
+  </si>
+  <si>
+    <t>femin</t>
+  </si>
+  <si>
+    <t>Pmax</t>
+  </si>
+  <si>
+    <t>Pmin</t>
+  </si>
+  <si>
+    <t>Ddn</t>
+  </si>
+  <si>
+    <t>Dup</t>
+  </si>
+  <si>
+    <t>REPCA1_1</t>
+  </si>
+  <si>
     <t>model</t>
   </si>
   <si>
@@ -580,9 +669,6 @@
   </si>
   <si>
     <t>Line</t>
-  </si>
-  <si>
-    <t>Vref1</t>
   </si>
 </sst>
 </file>
@@ -1484,6 +1570,74 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>0.02</v>
+      </c>
+      <c r="G2">
+        <v>0.02</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1513,52 +1667,52 @@
         <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>25</v>
@@ -1578,7 +1732,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -1646,13 +1800,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:BD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1671,70 +1825,70 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>86</v>
@@ -1743,88 +1897,88 @@
         <v>87</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.2">
@@ -1838,7 +1992,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1999,13 +2153,234 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2">
+        <v>0.02</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0.1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0.8</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0.01</v>
+      </c>
+      <c r="Q2">
+        <v>999</v>
+      </c>
+      <c r="R2">
+        <v>-999</v>
+      </c>
+      <c r="S2">
+        <v>-0.1</v>
+      </c>
+      <c r="T2">
+        <v>0.1</v>
+      </c>
+      <c r="U2">
+        <v>999</v>
+      </c>
+      <c r="V2">
+        <v>-999</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>0.1</v>
+      </c>
+      <c r="Y2">
+        <v>0.02</v>
+      </c>
+      <c r="Z2">
+        <v>-0.01</v>
+      </c>
+      <c r="AA2">
+        <v>0.01</v>
+      </c>
+      <c r="AB2">
+        <v>0.05</v>
+      </c>
+      <c r="AC2">
+        <v>-0.05</v>
+      </c>
+      <c r="AD2">
+        <v>999</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0.02</v>
+      </c>
+      <c r="AG2">
+        <v>0.05</v>
+      </c>
+      <c r="AH2">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2024,13 +2399,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2044,10 +2419,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>180</v>
+        <v>209</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
       <c r="F2" t="s">
         <v>51</v>
@@ -2067,10 +2442,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
       <c r="F3" t="s">
         <v>51</v>
@@ -2205,7 +2580,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Patched `s_update` when a lambda function returns a scalar; added REPCA1 calculations.
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_reg.xlsx
+++ b/andes/cases/kundur/kundur_reg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1E2AFB-0E64-2541-B46B-95BDB882981B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CEB2F8-7870-3A4D-8881-8B36C8F2379A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="7900" windowWidth="30260" windowHeight="19240" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4280" yWindow="2320" windowWidth="30260" windowHeight="19240" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -1572,7 +1572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
     </sheetView>
@@ -2157,9 +2157,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2307,12 +2307,6 @@
       </c>
       <c r="N2">
         <v>0.8</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0.01</v>
       </c>
       <c r="Q2">
         <v>999</v>

</xml_diff>

<commit_message>
`Model.s_update` now calls the lambdified and the numerical function for each service. Previously, lambdified calls and numerical calls were grouped respectively.
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_reg.xlsx
+++ b/andes/cases/kundur/kundur_reg.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CEB2F8-7870-3A4D-8881-8B36C8F2379A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="2320" windowWidth="30260" windowHeight="19240" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -28,12 +22,12 @@
     <sheet name="REPCA1" sheetId="13" r:id="rId13"/>
     <sheet name="Toggler" sheetId="14" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="215">
   <si>
     <t>idx</t>
   </si>
@@ -585,6 +579,15 @@
   </si>
   <si>
     <t>busf</t>
+  </si>
+  <si>
+    <t>VCFlag</t>
+  </si>
+  <si>
+    <t>RefFlag</t>
+  </si>
+  <si>
+    <t>Fflag</t>
   </si>
   <si>
     <t>Kp</t>
@@ -674,8 +677,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,14 +741,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -792,7 +787,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -824,27 +819,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -876,24 +853,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1069,17 +1028,517 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>1.1</v>
+      </c>
+      <c r="G2">
+        <v>0.9</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0.5702549171626017</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>1.1</v>
+      </c>
+      <c r="G3">
+        <v>0.9</v>
+      </c>
+      <c r="H3">
+        <v>0.99761</v>
+      </c>
+      <c r="I3">
+        <v>0.3687461830443478</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>1.1</v>
+      </c>
+      <c r="G4">
+        <v>0.9</v>
+      </c>
+      <c r="H4">
+        <v>0.96263</v>
+      </c>
+      <c r="I4">
+        <v>0.1853173146475028</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>1.1</v>
+      </c>
+      <c r="G5">
+        <v>0.9</v>
+      </c>
+      <c r="H5">
+        <v>0.81691</v>
+      </c>
+      <c r="I5">
+        <v>0.462358662804314</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>101</v>
+      </c>
+      <c r="E6">
+        <v>230</v>
+      </c>
+      <c r="F6">
+        <v>1.1</v>
+      </c>
+      <c r="G6">
+        <v>0.9</v>
+      </c>
+      <c r="H6">
+        <v>0.97928</v>
+      </c>
+      <c r="I6">
+        <v>0.4802029090767038</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>102</v>
+      </c>
+      <c r="E7">
+        <v>230</v>
+      </c>
+      <c r="F7">
+        <v>1.1</v>
+      </c>
+      <c r="G7">
+        <v>0.9</v>
+      </c>
+      <c r="H7">
+        <v>0.95796</v>
+      </c>
+      <c r="I7">
+        <v>0.2838865294831329</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>230</v>
+      </c>
+      <c r="F8">
+        <v>1.1</v>
+      </c>
+      <c r="G8">
+        <v>0.9</v>
+      </c>
+      <c r="H8">
+        <v>0.9362</v>
+      </c>
+      <c r="I8">
+        <v>0.1269011445832536</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>230</v>
+      </c>
+      <c r="F9">
+        <v>1.1</v>
+      </c>
+      <c r="G9">
+        <v>0.9</v>
+      </c>
+      <c r="H9">
+        <v>0.87904</v>
+      </c>
+      <c r="I9">
+        <v>-0.0805923235400888</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>112</v>
+      </c>
+      <c r="E10">
+        <v>230</v>
+      </c>
+      <c r="F10">
+        <v>1.1</v>
+      </c>
+      <c r="G10">
+        <v>0.9</v>
+      </c>
+      <c r="H10">
+        <v>0.89054</v>
+      </c>
+      <c r="I10">
+        <v>0.09361771574772226</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>111</v>
+      </c>
+      <c r="E11">
+        <v>230</v>
+      </c>
+      <c r="F11">
+        <v>1.1</v>
+      </c>
+      <c r="G11">
+        <v>0.9</v>
+      </c>
+      <c r="H11">
+        <v>0.82958</v>
+      </c>
+      <c r="I11">
+        <v>0.3366007088811167</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1093,506 +1552,6 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G2">
-        <v>0.9</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0.57025491716260168</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G3">
-        <v>0.9</v>
-      </c>
-      <c r="H3">
-        <v>0.99761</v>
-      </c>
-      <c r="I3">
-        <v>0.36874618304434781</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G4">
-        <v>0.9</v>
-      </c>
-      <c r="H4">
-        <v>0.96262999999999999</v>
-      </c>
-      <c r="I4">
-        <v>0.18531731464750281</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-      <c r="F5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G5">
-        <v>0.9</v>
-      </c>
-      <c r="H5">
-        <v>0.81691000000000003</v>
-      </c>
-      <c r="I5">
-        <v>0.46235866280431398</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>2</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>101</v>
-      </c>
-      <c r="E6">
-        <v>230</v>
-      </c>
-      <c r="F6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G6">
-        <v>0.9</v>
-      </c>
-      <c r="H6">
-        <v>0.97928000000000004</v>
-      </c>
-      <c r="I6">
-        <v>0.48020290907670382</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>102</v>
-      </c>
-      <c r="E7">
-        <v>230</v>
-      </c>
-      <c r="F7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G7">
-        <v>0.9</v>
-      </c>
-      <c r="H7">
-        <v>0.95796000000000003</v>
-      </c>
-      <c r="I7">
-        <v>0.28388652948313292</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>230</v>
-      </c>
-      <c r="F8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G8">
-        <v>0.9</v>
-      </c>
-      <c r="H8">
-        <v>0.93620000000000003</v>
-      </c>
-      <c r="I8">
-        <v>0.12690114458325361</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>13</v>
-      </c>
-      <c r="E9">
-        <v>230</v>
-      </c>
-      <c r="F9">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G9">
-        <v>0.9</v>
-      </c>
-      <c r="H9">
-        <v>0.87904000000000004</v>
-      </c>
-      <c r="I9">
-        <v>-8.0592323540088801E-2</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>2</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>112</v>
-      </c>
-      <c r="E10">
-        <v>230</v>
-      </c>
-      <c r="F10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G10">
-        <v>0.9</v>
-      </c>
-      <c r="H10">
-        <v>0.89054</v>
-      </c>
-      <c r="I10">
-        <v>9.3617715747722263E-2</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>2</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>111</v>
-      </c>
-      <c r="E11">
-        <v>230</v>
-      </c>
-      <c r="F11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G11">
-        <v>0.9</v>
-      </c>
-      <c r="H11">
-        <v>0.82957999999999998</v>
-      </c>
-      <c r="I11">
-        <v>0.33660070888111671</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>2</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1605,7 +1564,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1637,7 +1596,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1645,9 +1604,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1721,7 +1680,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1801,7 +1760,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1809,9 +1768,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:56">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1981,7 +1940,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:56">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2016,7 +1975,7 @@
         <v>0.96</v>
       </c>
       <c r="M2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="N2">
         <v>0.02</v>
@@ -2154,17 +2113,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:AH2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2190,16 +2149,16 @@
         <v>183</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>187</v>
@@ -2220,34 +2179,34 @@
         <v>192</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>196</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>200</v>
@@ -2259,16 +2218,25 @@
         <v>202</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AJ1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2279,7 +2247,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2291,75 +2259,84 @@
         <v>113</v>
       </c>
       <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>0.02</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
         <v>0.1</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
         <v>0.8</v>
       </c>
-      <c r="Q2">
+      <c r="T2">
         <v>999</v>
       </c>
-      <c r="R2">
+      <c r="U2">
         <v>-999</v>
       </c>
-      <c r="S2">
+      <c r="V2">
         <v>-0.1</v>
       </c>
-      <c r="T2">
+      <c r="W2">
         <v>0.1</v>
       </c>
-      <c r="U2">
+      <c r="X2">
         <v>999</v>
       </c>
-      <c r="V2">
+      <c r="Y2">
         <v>-999</v>
       </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="X2">
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
         <v>0.1</v>
       </c>
-      <c r="Y2">
+      <c r="AB2">
         <v>0.02</v>
       </c>
-      <c r="Z2">
+      <c r="AC2">
         <v>-0.01</v>
       </c>
-      <c r="AA2">
+      <c r="AD2">
         <v>0.01</v>
       </c>
-      <c r="AB2">
+      <c r="AE2">
         <v>0.05</v>
       </c>
-      <c r="AC2">
+      <c r="AF2">
         <v>-0.05</v>
       </c>
-      <c r="AD2">
+      <c r="AG2">
         <v>999</v>
       </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
         <v>0.02</v>
       </c>
-      <c r="AG2">
+      <c r="AJ2">
         <v>0.05</v>
       </c>
-      <c r="AH2">
+      <c r="AK2">
         <v>0.05</v>
       </c>
     </row>
@@ -2369,7 +2346,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2377,9 +2354,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2393,16 +2370,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2413,10 +2390,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F2" t="s">
         <v>51</v>
@@ -2425,7 +2402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2436,10 +2413,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E3" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F3" t="s">
         <v>51</v>
@@ -2454,7 +2431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2462,9 +2439,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2499,7 +2476,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2519,10 +2496,10 @@
         <v>11.59</v>
       </c>
       <c r="H2">
-        <v>-0.73499999999999999</v>
+        <v>-0.735</v>
       </c>
       <c r="I2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J2">
         <v>0.9</v>
@@ -2531,7 +2508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2551,10 +2528,10 @@
         <v>15.75</v>
       </c>
       <c r="H3">
-        <v>-0.89900000000000002</v>
+        <v>-0.899</v>
       </c>
       <c r="I3">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J3">
         <v>0.9</v>
@@ -2569,7 +2546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2577,9 +2554,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2638,7 +2615,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2691,7 +2668,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2744,7 +2721,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2803,7 +2780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2811,9 +2788,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2875,7 +2852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2895,10 +2872,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>7.4586100000000002</v>
+        <v>7.45861</v>
       </c>
       <c r="J2">
-        <v>1.4361200000000001</v>
+        <v>1.43612</v>
       </c>
       <c r="K2">
         <v>9</v>
@@ -2928,7 +2905,7 @@
         <v>0.25</v>
       </c>
       <c r="T2">
-        <v>0.57025491716260168</v>
+        <v>0.5702549171626017</v>
       </c>
     </row>
   </sheetData>
@@ -2937,7 +2914,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2945,9 +2922,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3021,7 +2998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3050,13 +3027,13 @@
         <v>230</v>
       </c>
       <c r="K2">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="L2">
         <v>0.05</v>
       </c>
       <c r="M2">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -3083,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3112,13 +3089,13 @@
         <v>230</v>
       </c>
       <c r="K3">
-        <v>5.0099999999999997E-3</v>
+        <v>0.00501</v>
       </c>
       <c r="L3">
-        <v>5.0009999999999999E-2</v>
+        <v>0.05001</v>
       </c>
       <c r="M3">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -3145,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3174,7 +3151,7 @@
         <v>230</v>
       </c>
       <c r="K4">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="L4">
         <v>0.02</v>
@@ -3207,7 +3184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3236,10 +3213,10 @@
         <v>230</v>
       </c>
       <c r="K5">
-        <v>2.0100000000000001E-3</v>
+        <v>0.00201</v>
       </c>
       <c r="L5">
-        <v>2.001E-2</v>
+        <v>0.02001</v>
       </c>
       <c r="M5">
         <v>0.03</v>
@@ -3269,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3298,10 +3275,10 @@
         <v>230</v>
       </c>
       <c r="K6">
-        <v>2.2009999999999998E-2</v>
+        <v>0.02201</v>
       </c>
       <c r="L6">
-        <v>0.22001000000000001</v>
+        <v>0.22001</v>
       </c>
       <c r="M6">
         <v>0.33</v>
@@ -3331,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3360,10 +3337,10 @@
         <v>230</v>
       </c>
       <c r="K7">
-        <v>2.2020000000000001E-2</v>
+        <v>0.02202</v>
       </c>
       <c r="L7">
-        <v>0.22001999999999999</v>
+        <v>0.22002</v>
       </c>
       <c r="M7">
         <v>0.33</v>
@@ -3393,7 +3370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3422,7 +3399,7 @@
         <v>230</v>
       </c>
       <c r="K8">
-        <v>2.1999999999999999E-2</v>
+        <v>0.022</v>
       </c>
       <c r="L8">
         <v>0.22</v>
@@ -3455,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3484,7 +3461,7 @@
         <v>230</v>
       </c>
       <c r="K9">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="L9">
         <v>0.02</v>
@@ -3517,7 +3494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3546,10 +3523,10 @@
         <v>230</v>
       </c>
       <c r="K10">
-        <v>2.0100000000000001E-3</v>
+        <v>0.00201</v>
       </c>
       <c r="L10">
-        <v>2.001E-2</v>
+        <v>0.02001</v>
       </c>
       <c r="M10">
         <v>0.03</v>
@@ -3579,7 +3556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3608,13 +3585,13 @@
         <v>230</v>
       </c>
       <c r="K11">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="L11">
         <v>0.05</v>
       </c>
       <c r="M11">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -3641,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3670,13 +3647,13 @@
         <v>230</v>
       </c>
       <c r="K12">
-        <v>5.0099999999999997E-3</v>
+        <v>0.00501</v>
       </c>
       <c r="L12">
-        <v>5.0009999999999999E-2</v>
+        <v>0.05001</v>
       </c>
       <c r="M12">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -3703,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3732,10 +3709,10 @@
         <v>230</v>
       </c>
       <c r="K13">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L13">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -3765,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3794,10 +3771,10 @@
         <v>230</v>
       </c>
       <c r="K14">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L14">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -3827,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3856,10 +3833,10 @@
         <v>230</v>
       </c>
       <c r="K15">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L15">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -3889,7 +3866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3918,10 +3895,10 @@
         <v>230</v>
       </c>
       <c r="K16">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L16">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -3957,7 +3934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3965,9 +3942,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3981,7 +3958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3995,7 +3972,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4015,7 +3992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4023,9 +4000,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -4111,7 +4088,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4176,7 +4153,7 @@
         <v>0.25</v>
       </c>
       <c r="W2">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X2">
         <v>0.25</v>
@@ -4194,7 +4171,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4259,7 +4236,7 @@
         <v>0.25</v>
       </c>
       <c r="W3">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X3">
         <v>0.25</v>
@@ -4277,7 +4254,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4342,7 +4319,7 @@
         <v>0.25</v>
       </c>
       <c r="W4">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X4">
         <v>0.25</v>
@@ -4366,7 +4343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4374,9 +4351,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -4420,7 +4397,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4461,7 +4438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4502,7 +4479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4549,7 +4526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4557,9 +4534,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -4621,7 +4598,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4656,7 +4633,7 @@
         <v>1.246</v>
       </c>
       <c r="L2">
-        <v>7.5399999999999995E-2</v>
+        <v>0.07539999999999999</v>
       </c>
       <c r="M2">
         <v>20</v>
@@ -4683,7 +4660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4718,7 +4695,7 @@
         <v>1.246</v>
       </c>
       <c r="L3">
-        <v>7.5399999999999995E-2</v>
+        <v>0.07539999999999999</v>
       </c>
       <c r="M3">
         <v>20</v>
@@ -4745,7 +4722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4780,7 +4757,7 @@
         <v>1.246</v>
       </c>
       <c r="L4">
-        <v>7.5399999999999995E-2</v>
+        <v>0.07539999999999999</v>
       </c>
       <c r="M4">
         <v>20</v>

</xml_diff>

<commit_message>
Updated `kundur_reg.xlsx`; minor tweaks to `s_update_var`
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_reg.xlsx
+++ b/andes/cases/kundur/kundur_reg.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4661245B-02E2-4B4F-905F-51AC78C814E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="31640" yWindow="160" windowWidth="32600" windowHeight="18620" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -22,12 +28,12 @@
     <sheet name="REPCA1" sheetId="13" r:id="rId13"/>
     <sheet name="Toggler" sheetId="14" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="216">
   <si>
     <t>idx</t>
   </si>
@@ -672,13 +678,16 @@
   </si>
   <si>
     <t>Line</t>
+  </si>
+  <si>
+    <t>Kc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,6 +750,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -787,7 +804,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -819,9 +836,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -853,6 +888,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1028,17 +1081,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1082,7 +1135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1099,7 +1152,7 @@
         <v>20</v>
       </c>
       <c r="F2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G2">
         <v>0.9</v>
@@ -1108,7 +1161,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0.5702549171626017</v>
+        <v>0.57025491716260168</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -1126,7 +1179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1143,7 +1196,7 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G3">
         <v>0.9</v>
@@ -1152,7 +1205,7 @@
         <v>0.99761</v>
       </c>
       <c r="I3">
-        <v>0.3687461830443478</v>
+        <v>0.36874618304434781</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1170,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1187,16 +1240,16 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G4">
         <v>0.9</v>
       </c>
       <c r="H4">
-        <v>0.96263</v>
+        <v>0.96262999999999999</v>
       </c>
       <c r="I4">
-        <v>0.1853173146475028</v>
+        <v>0.18531731464750281</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1214,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1231,16 +1284,16 @@
         <v>20</v>
       </c>
       <c r="F5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G5">
         <v>0.9</v>
       </c>
       <c r="H5">
-        <v>0.81691</v>
+        <v>0.81691000000000003</v>
       </c>
       <c r="I5">
-        <v>0.462358662804314</v>
+        <v>0.46235866280431398</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1258,7 +1311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1275,16 +1328,16 @@
         <v>230</v>
       </c>
       <c r="F6">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G6">
         <v>0.9</v>
       </c>
       <c r="H6">
-        <v>0.97928</v>
+        <v>0.97928000000000004</v>
       </c>
       <c r="I6">
-        <v>0.4802029090767038</v>
+        <v>0.48020290907670382</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1302,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1319,16 +1372,16 @@
         <v>230</v>
       </c>
       <c r="F7">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G7">
         <v>0.9</v>
       </c>
       <c r="H7">
-        <v>0.95796</v>
+        <v>0.95796000000000003</v>
       </c>
       <c r="I7">
-        <v>0.2838865294831329</v>
+        <v>0.28388652948313292</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1346,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1363,16 +1416,16 @@
         <v>230</v>
       </c>
       <c r="F8">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G8">
         <v>0.9</v>
       </c>
       <c r="H8">
-        <v>0.9362</v>
+        <v>0.93620000000000003</v>
       </c>
       <c r="I8">
-        <v>0.1269011445832536</v>
+        <v>0.12690114458325361</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1390,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1407,16 +1460,16 @@
         <v>230</v>
       </c>
       <c r="F9">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G9">
         <v>0.9</v>
       </c>
       <c r="H9">
-        <v>0.87904</v>
+        <v>0.87904000000000004</v>
       </c>
       <c r="I9">
-        <v>-0.0805923235400888</v>
+        <v>-8.0592323540088801E-2</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1434,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1451,7 +1504,7 @@
         <v>230</v>
       </c>
       <c r="F10">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G10">
         <v>0.9</v>
@@ -1460,7 +1513,7 @@
         <v>0.89054</v>
       </c>
       <c r="I10">
-        <v>0.09361771574772226</v>
+        <v>9.3617715747722263E-2</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1478,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1495,16 +1548,16 @@
         <v>230</v>
       </c>
       <c r="F11">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G11">
         <v>0.9</v>
       </c>
       <c r="H11">
-        <v>0.82958</v>
+        <v>0.82957999999999998</v>
       </c>
       <c r="I11">
-        <v>0.3366007088811167</v>
+        <v>0.33660070888111671</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1528,7 +1581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1536,9 +1589,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1564,7 +1617,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1596,7 +1649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1604,9 +1657,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1680,7 +1733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1760,7 +1813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:BD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1768,9 +1821,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:56">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1940,7 +1993,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:56">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1975,7 +2028,7 @@
         <v>0.96</v>
       </c>
       <c r="M2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N2">
         <v>0.02</v>
@@ -2113,17 +2166,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2182,61 +2235,64 @@
         <v>193</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2259,10 +2315,10 @@
         <v>113</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2283,61 +2339,64 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>0.8</v>
+        <v>0.98</v>
       </c>
       <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
         <v>999</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>-999</v>
       </c>
-      <c r="V2">
-        <v>-0.1</v>
-      </c>
       <c r="W2">
+        <v>-0.02</v>
+      </c>
+      <c r="X2">
+        <v>0.02</v>
+      </c>
+      <c r="Y2">
+        <v>999</v>
+      </c>
+      <c r="Z2">
+        <v>-999</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
         <v>0.1</v>
       </c>
-      <c r="X2">
+      <c r="AC2">
+        <v>0.02</v>
+      </c>
+      <c r="AD2">
+        <v>-0.01</v>
+      </c>
+      <c r="AE2">
+        <v>0.01</v>
+      </c>
+      <c r="AF2">
+        <v>0.05</v>
+      </c>
+      <c r="AG2">
+        <v>-0.05</v>
+      </c>
+      <c r="AH2">
         <v>999</v>
       </c>
-      <c r="Y2">
+      <c r="AI2">
         <v>-999</v>
       </c>
-      <c r="Z2">
-        <v>1</v>
-      </c>
-      <c r="AA2">
-        <v>0.1</v>
-      </c>
-      <c r="AB2">
+      <c r="AJ2">
         <v>0.02</v>
       </c>
-      <c r="AC2">
-        <v>-0.01</v>
-      </c>
-      <c r="AD2">
-        <v>0.01</v>
-      </c>
-      <c r="AE2">
-        <v>0.05</v>
-      </c>
-      <c r="AF2">
-        <v>-0.05</v>
-      </c>
-      <c r="AG2">
-        <v>999</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>0.02</v>
-      </c>
-      <c r="AJ2">
-        <v>0.05</v>
-      </c>
       <c r="AK2">
-        <v>0.05</v>
+        <v>10</v>
+      </c>
+      <c r="AL2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2346,17 +2405,17 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2379,7 +2438,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2402,7 +2461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2410,7 +2469,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>213</v>
@@ -2431,7 +2490,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2439,9 +2498,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2476,7 +2535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2496,10 +2555,10 @@
         <v>11.59</v>
       </c>
       <c r="H2">
-        <v>-0.735</v>
+        <v>-0.73499999999999999</v>
       </c>
       <c r="I2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J2">
         <v>0.9</v>
@@ -2508,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2528,10 +2587,10 @@
         <v>15.75</v>
       </c>
       <c r="H3">
-        <v>-0.899</v>
+        <v>-0.89900000000000002</v>
       </c>
       <c r="I3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J3">
         <v>0.9</v>
@@ -2546,7 +2605,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2554,9 +2613,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2615,7 +2674,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2668,7 +2727,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2721,7 +2780,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2780,7 +2839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2788,9 +2847,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2852,7 +2911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2872,10 +2931,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>7.45861</v>
+        <v>7.4586100000000002</v>
       </c>
       <c r="J2">
-        <v>1.43612</v>
+        <v>1.4361200000000001</v>
       </c>
       <c r="K2">
         <v>9</v>
@@ -2905,7 +2964,7 @@
         <v>0.25</v>
       </c>
       <c r="T2">
-        <v>0.5702549171626017</v>
+        <v>0.57025491716260168</v>
       </c>
     </row>
   </sheetData>
@@ -2914,7 +2973,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2922,9 +2981,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2998,7 +3057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3027,13 +3086,13 @@
         <v>230</v>
       </c>
       <c r="K2">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="L2">
         <v>0.05</v>
       </c>
       <c r="M2">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -3060,7 +3119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3089,13 +3148,13 @@
         <v>230</v>
       </c>
       <c r="K3">
-        <v>0.00501</v>
+        <v>5.0099999999999997E-3</v>
       </c>
       <c r="L3">
-        <v>0.05001</v>
+        <v>5.0009999999999999E-2</v>
       </c>
       <c r="M3">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -3122,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3151,7 +3210,7 @@
         <v>230</v>
       </c>
       <c r="K4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="L4">
         <v>0.02</v>
@@ -3184,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3213,10 +3272,10 @@
         <v>230</v>
       </c>
       <c r="K5">
-        <v>0.00201</v>
+        <v>2.0100000000000001E-3</v>
       </c>
       <c r="L5">
-        <v>0.02001</v>
+        <v>2.001E-2</v>
       </c>
       <c r="M5">
         <v>0.03</v>
@@ -3246,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3275,10 +3334,10 @@
         <v>230</v>
       </c>
       <c r="K6">
-        <v>0.02201</v>
+        <v>2.2009999999999998E-2</v>
       </c>
       <c r="L6">
-        <v>0.22001</v>
+        <v>0.22001000000000001</v>
       </c>
       <c r="M6">
         <v>0.33</v>
@@ -3308,7 +3367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3337,10 +3396,10 @@
         <v>230</v>
       </c>
       <c r="K7">
-        <v>0.02202</v>
+        <v>2.2020000000000001E-2</v>
       </c>
       <c r="L7">
-        <v>0.22002</v>
+        <v>0.22001999999999999</v>
       </c>
       <c r="M7">
         <v>0.33</v>
@@ -3370,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3399,7 +3458,7 @@
         <v>230</v>
       </c>
       <c r="K8">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="L8">
         <v>0.22</v>
@@ -3432,7 +3491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3461,7 +3520,7 @@
         <v>230</v>
       </c>
       <c r="K9">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="L9">
         <v>0.02</v>
@@ -3494,7 +3553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3523,10 +3582,10 @@
         <v>230</v>
       </c>
       <c r="K10">
-        <v>0.00201</v>
+        <v>2.0100000000000001E-3</v>
       </c>
       <c r="L10">
-        <v>0.02001</v>
+        <v>2.001E-2</v>
       </c>
       <c r="M10">
         <v>0.03</v>
@@ -3556,7 +3615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3585,13 +3644,13 @@
         <v>230</v>
       </c>
       <c r="K11">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="L11">
         <v>0.05</v>
       </c>
       <c r="M11">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -3618,7 +3677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3647,13 +3706,13 @@
         <v>230</v>
       </c>
       <c r="K12">
-        <v>0.00501</v>
+        <v>5.0099999999999997E-3</v>
       </c>
       <c r="L12">
-        <v>0.05001</v>
+        <v>5.0009999999999999E-2</v>
       </c>
       <c r="M12">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -3680,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3709,10 +3768,10 @@
         <v>230</v>
       </c>
       <c r="K13">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L13">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -3742,7 +3801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3771,10 +3830,10 @@
         <v>230</v>
       </c>
       <c r="K14">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L14">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -3804,7 +3863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3833,10 +3892,10 @@
         <v>230</v>
       </c>
       <c r="K15">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L15">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -3866,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3895,10 +3954,10 @@
         <v>230</v>
       </c>
       <c r="K16">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L16">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -3934,7 +3993,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3942,9 +4001,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3958,7 +4017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3972,7 +4031,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3992,7 +4051,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4000,9 +4059,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -4088,7 +4147,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4153,7 +4212,7 @@
         <v>0.25</v>
       </c>
       <c r="W2">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X2">
         <v>0.25</v>
@@ -4171,7 +4230,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4236,7 +4295,7 @@
         <v>0.25</v>
       </c>
       <c r="W3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X3">
         <v>0.25</v>
@@ -4254,7 +4313,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4319,7 +4378,7 @@
         <v>0.25</v>
       </c>
       <c r="W4">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X4">
         <v>0.25</v>
@@ -4343,7 +4402,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4351,9 +4410,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -4397,7 +4456,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4438,7 +4497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4479,7 +4538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4526,7 +4585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4534,9 +4593,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -4598,7 +4657,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4633,7 +4692,7 @@
         <v>1.246</v>
       </c>
       <c r="L2">
-        <v>0.07539999999999999</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M2">
         <v>20</v>
@@ -4660,7 +4719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4695,7 +4754,7 @@
         <v>1.246</v>
       </c>
       <c r="L3">
-        <v>0.07539999999999999</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M3">
         <v>20</v>
@@ -4722,7 +4781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4757,7 +4816,7 @@
         <v>1.246</v>
       </c>
       <c r="L4">
-        <v>0.07539999999999999</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M4">
         <v>20</v>

</xml_diff>

<commit_message>
Updated renewable test case.
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_reg.xlsx
+++ b/andes/cases/kundur/kundur_reg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD0F6BB-B35C-CD41-978D-B34874B25055}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E103182A-20A3-A14B-87CA-327C57CD49F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="6400" windowWidth="30060" windowHeight="20440" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="460" windowWidth="30060" windowHeight="19420" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="221">
   <si>
     <t>idx</t>
   </si>
@@ -1832,7 +1832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:BD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U2" sqref="U2"/>
     </sheetView>
@@ -2424,7 +2424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
@@ -2458,11 +2458,11 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>213</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>213</v>
@@ -2474,18 +2474,18 @@
         <v>51</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>214</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>214</v>
@@ -2497,7 +2497,7 @@
         <v>51</v>
       </c>
       <c r="G3">
-        <v>2.1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2511,7 +2511,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2549,11 +2549,11 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>220</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>220</v>
@@ -2562,10 +2562,10 @@
         <v>8</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>2.1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>